<commit_message>
TOP-00 From SC to CC
</commit_message>
<xml_diff>
--- a/src/coursera_Python.xlsx
+++ b/src/coursera_Python.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,221 +463,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Crash Course on Python</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Google</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Skills you'll gain: Computer Programming, Data Structures, Problem Solving, Python Programming</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">4.8
-</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>35K reviews</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Beginner</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Course</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>1 - 3 Months</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Python Basics</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>University of Michigan</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Skills you'll gain: Computer Programming, Python Programming, Problem Solving</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">4.8
-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>17K reviews</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Beginner</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Course</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>1 - 4 Weeks</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Data Analysis with Python</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>IBM</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Skills you'll gain: Python Programming, Data Analysis, Machine Learning, Computer Programming, Exploratory Data Analysis, General Statistics, Machine Learning Algorithms, Plot (Graphics), Probability &amp; Statistics, Regression, Statistical Programming</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">4.7
-</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>17K reviews</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Beginner</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Course</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1 - 3 Months</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Programming in Python</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Meta</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Skills you'll gain: Python Programming, Programming Principles, Big Data, Software Testing, Algorithms, Computer Programming, Django (Web Framework), Tensorflow</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">4.7
-</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1.2K reviews</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Beginner</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Course</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>1 - 3 Months</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Learn to Program: The Fundamentals</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>University of Toronto</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Skills you'll gain: Computer Programming, Python Programming, Computational Logic, Problem Solving, Programming Principles, Computer Programming Tools, Critical Thinking, Computational Thinking, Mathematics, Process Analysis</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">4.7
-</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>6.3K reviews</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Beginner</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Course</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>1 - 3 Months</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>